<commit_message>
feat: adiciona suporte a expand_dates_to para transformar colunas de data em Ano, Mes e Valor
</commit_message>
<xml_diff>
--- a/schema-checker/data/inputs/xlsx/sample.xlsx
+++ b/schema-checker/data/inputs/xlsx/sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID da Pesquisa</t>
   </si>
@@ -27,6 +27,12 @@
   </si>
   <si>
     <t>Aleatorio</t>
+  </si>
+  <si>
+    <t>30/11/20</t>
+  </si>
+  <si>
+    <t>30/04/20</t>
   </si>
   <si>
     <t>kaxy</t>
@@ -355,56 +361,80 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
         <v>0.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>0.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.08</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>0.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -424,13 +454,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>